<commit_message>
Fix small typo. Need to regen csv
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="6975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="6975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016Names" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>peter wolfe</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -577,9 +577,6 @@
     <t xml:space="preserve">Don't half-ass anything. Whatever you do, use you full ass. </t>
   </si>
   <si>
-    <t>A little progress each day adds up</t>
-  </si>
-  <si>
     <t>You will never have this day again. Make it count.</t>
   </si>
   <si>
@@ -610,13 +607,7 @@
     <t>Dreams don't work unless you do</t>
   </si>
   <si>
-    <t>Work hard so that someday you signature will be called an autograph</t>
-  </si>
-  <si>
     <t>Be so good they cannot ignore you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">don't stope when you are tired. Stop when you are done. </t>
   </si>
   <si>
     <t>OK people. Let's do this!</t>
@@ -779,9 +770,6 @@
     <t>You can stay but your clothes must go...</t>
   </si>
   <si>
-    <t>All that awesome is such a little boy...</t>
-  </si>
-  <si>
     <t>Goodbyes are not forever, 
 Goodbyes are not the end. 
 They simply mean I'll miss you, 
@@ -789,11 +777,6 @@
   </si>
   <si>
     <t>Don't cry because it's over, smile because it happened.</t>
-  </si>
-  <si>
-    <t>We'll meet again, 
-Don't know where,Don't know when, 
-But I know we’ll meet again, some sunny day.</t>
   </si>
   <si>
     <t xml:space="preserve">Being positive in a negative situation is not naive. It's leadership. </t>
@@ -808,11 +791,28 @@
   <si>
     <t>Goodbyes make you think. They make you realize what you've had, what you've lost, and what you've taken for granted.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Don't stop when you are tired. Stop when you are done. </t>
+  </si>
+  <si>
+    <t>Work hard so that someday your signature will be called an autograph</t>
+  </si>
+  <si>
+    <t>We'll meet again, 
+Don't know where, Don't know when, 
+But I know we’ll meet again, some sunny day.</t>
+  </si>
+  <si>
+    <t>A little progress each day adds up.</t>
+  </si>
+  <si>
+    <t>All that awesome in such a little boy...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="10"/>
@@ -900,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -934,6 +934,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,12 +1251,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1293,7 +1296,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75">
-      <c r="A3" s="3">
+      <c r="A3" s="18">
         <v>49550490</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1444,10 +1447,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12.75">
@@ -1458,10 +1461,10 @@
         <v>111</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.75">
@@ -1472,10 +1475,10 @@
         <v>26</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12.75">
@@ -1486,10 +1489,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75">
@@ -1500,10 +1503,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75">
@@ -1517,7 +1520,7 @@
         <v>138</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75">
@@ -1531,7 +1534,7 @@
         <v>155</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="63.75">
@@ -1542,10 +1545,10 @@
         <v>29</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75">
@@ -1556,10 +1559,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25">
@@ -1573,7 +1576,7 @@
         <v>157</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51">
@@ -1584,10 +1587,10 @@
         <v>114</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75">
@@ -1598,10 +1601,10 @@
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75">
@@ -1615,7 +1618,7 @@
         <v>137</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="12.75">
@@ -1629,7 +1632,7 @@
         <v>139</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75">
@@ -1640,10 +1643,10 @@
         <v>116</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12.75">
@@ -1668,7 +1671,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>160</v>
@@ -1682,10 +1685,10 @@
         <v>24</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="51">
@@ -1699,7 +1702,7 @@
         <v>167</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="12.75">
@@ -1713,7 +1716,7 @@
         <v>161</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="12.75">
@@ -1727,7 +1730,7 @@
         <v>154</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="12.75">
@@ -1741,7 +1744,7 @@
         <v>162</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="12.75">
@@ -1752,10 +1755,10 @@
         <v>120</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="12.75">
@@ -1766,10 +1769,10 @@
         <v>30</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="12.75">
@@ -1780,10 +1783,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12.75">
@@ -1797,7 +1800,7 @@
         <v>164</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="12.75">
@@ -1808,10 +1811,10 @@
         <v>121</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.75">
@@ -1822,10 +1825,10 @@
         <v>122</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="12.75">
@@ -1839,7 +1842,7 @@
         <v>163</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="12.75">
@@ -1853,7 +1856,7 @@
         <v>165</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="12.75">
@@ -1867,7 +1870,7 @@
         <v>139</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12.75">
@@ -1881,7 +1884,7 @@
         <v>168</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12.75">
@@ -1895,7 +1898,7 @@
         <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.75">
@@ -1906,10 +1909,10 @@
         <v>126</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12.75">
@@ -1920,10 +1923,10 @@
         <v>125</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12.75">
@@ -1934,7 +1937,7 @@
         <v>25</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>166</v>
@@ -1951,7 +1954,7 @@
         <v>170</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="12.75">
@@ -1965,7 +1968,7 @@
         <v>171</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.75">
@@ -1976,10 +1979,10 @@
         <v>21</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="12.75">
@@ -1993,7 +1996,7 @@
         <v>172</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.75">
@@ -2007,7 +2010,7 @@
         <v>173</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="63.75">
@@ -2018,10 +2021,10 @@
         <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12.75">
@@ -2032,10 +2035,10 @@
         <v>129</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12.75">
@@ -2046,10 +2049,10 @@
         <v>13</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12.75">
@@ -2060,10 +2063,10 @@
         <v>130</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12.75">
@@ -2074,10 +2077,10 @@
         <v>131</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.75">
@@ -2088,10 +2091,10 @@
         <v>11</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12.75">
@@ -2102,10 +2105,10 @@
         <v>132</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="12.75">
@@ -2114,7 +2117,7 @@
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Fix UTF-16 issue. File redirection from java to System.stdout is apparently ALWAYS UTF-16. Tried 50 different things and couldn't fix it so gave up and just always write to ./sync/current.csv. Lame. Need to enhance to take an output filename.
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="6975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="6975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016Names" sheetId="2" r:id="rId1"/>
     <sheet name="Avail. Tags" sheetId="4" r:id="rId2"/>
-    <sheet name="Lost or broken tags" sheetId="3" r:id="rId3"/>
-    <sheet name="Unused hello-goodbye" sheetId="5" r:id="rId4"/>
+    <sheet name="tags to give out" sheetId="6" r:id="rId3"/>
+    <sheet name="Lost or broken tags" sheetId="3" r:id="rId4"/>
+    <sheet name="Unused hello-goodbye" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2016Names'!$A$1:$D$1</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="353">
   <si>
     <t>RFID</t>
   </si>
@@ -1117,6 +1118,36 @@
   </si>
   <si>
     <t>See you later alligator!</t>
+  </si>
+  <si>
+    <t>Joy Wolfe</t>
+  </si>
+  <si>
+    <t>Mrs Young</t>
+  </si>
+  <si>
+    <t>Mr. Young</t>
+  </si>
+  <si>
+    <t>Mr. Borowski</t>
+  </si>
+  <si>
+    <t>Nick Anderson</t>
+  </si>
+  <si>
+    <t>peter matthews</t>
+  </si>
+  <si>
+    <t>amanda quon</t>
+  </si>
+  <si>
+    <t>nolan quon</t>
+  </si>
+  <si>
+    <t>julia ruch</t>
+  </si>
+  <si>
+    <t>aneesh</t>
   </si>
 </sst>
 </file>
@@ -1595,9 +1626,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2592,7 +2623,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2608,38 +2639,6 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>40</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>45</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>74</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="6" spans="1:2">
       <c r="A6">
         <v>77</v>
@@ -2664,60 +2663,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>81</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="10" spans="1:2">
       <c r="A10">
         <v>113</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>114</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>125</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>126</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>128</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>134</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5">
@@ -2742,6 +2693,134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90371E08-1F3F-42FF-B479-1FD1C921154F}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>18</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>40</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>74</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>81</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>114</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>125</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>126</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>134</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927B54C8-D484-4F95-9F62-7C995A45FCA6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2781,7 +2860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B571F4-9364-46F7-82CE-0B9371F3638F}">
   <dimension ref="A1:B33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updates for 2020 barcode support
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\wolfe\Documents\Misc\Personal\transfer\FIRST\Github\rfid_reader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E455C84-91E0-4C92-8693-8D254D8796E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972FEE58-190B-4B73-A7C8-493BA2FA840F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="810" windowWidth="28360" windowHeight="20310" tabRatio="682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="485">
   <si>
     <t>RFID</t>
   </si>
@@ -1584,6 +1584,9 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>X002AZOCAN</t>
   </si>
 </sst>
 </file>
@@ -2123,7 +2126,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -2894,9 +2897,8 @@
       <c r="A43" s="16">
         <v>49550490</v>
       </c>
-      <c r="B43" s="39" t="str">
-        <f>IF(ISNA(VLOOKUP(C43, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C43, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+      <c r="B43" s="39">
+        <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>15</v>
@@ -2912,8 +2914,8 @@
       <c r="A44" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B44" s="39">
-        <v>99</v>
+      <c r="B44" s="39" t="s">
+        <v>484</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Don't echo the barcodes!!! Update the csv file with kevin/connie ids
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\wolfe\Documents\Misc\Personal\transfer\FIRST\Github\rfid_reader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972FEE58-190B-4B73-A7C8-493BA2FA840F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663E5AD-C2FA-4EDE-B2BC-38C638B6CCEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="810" windowWidth="28360" windowHeight="20310" tabRatio="682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="487">
   <si>
     <t>RFID</t>
   </si>
@@ -1587,6 +1587,12 @@
   </si>
   <si>
     <t>X002AZOCAN</t>
+  </si>
+  <si>
+    <t>23OttoK@rvilleschools.org</t>
+  </si>
+  <si>
+    <t>constancemehl@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2126,7 +2132,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5"/>
@@ -2645,9 +2651,9 @@
       <c r="A29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="39" t="str">
+      <c r="B29" s="39">
         <f>IF(ISNA(VLOOKUP(C29, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C29, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>200266</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>62</v>
@@ -3201,9 +3207,9 @@
       <c r="A60" t="s">
         <v>333</v>
       </c>
-      <c r="B60" s="39" t="str">
+      <c r="B60" s="39">
         <f>IF(ISNA(VLOOKUP(C60, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C60, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>230116</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>371</v>
@@ -3406,11 +3412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F719BBFE-2A3C-4504-AB28-C8BF6B3B6524}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3439,7 +3444,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="2" spans="1:5" ht="13" thickBot="1">
       <c r="A2" s="42">
         <v>43811.747175925928</v>
       </c>
@@ -3456,7 +3461,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="3" spans="1:5" ht="13" thickBot="1">
       <c r="A3" s="42">
         <v>43811.304988425924</v>
       </c>
@@ -3473,7 +3478,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="4" spans="1:5" ht="13" thickBot="1">
       <c r="A4" s="42">
         <v>43813.510659722226</v>
       </c>
@@ -3490,7 +3495,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="5" spans="1:5" ht="13" thickBot="1">
       <c r="A5" s="42">
         <v>43810.982511574075</v>
       </c>
@@ -3507,7 +3512,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="6" spans="1:5" ht="13" thickBot="1">
       <c r="A6" s="42">
         <v>43811.577881944446</v>
       </c>
@@ -3558,7 +3563,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="9" spans="1:5" ht="13" thickBot="1">
       <c r="A9" s="42">
         <v>43811.943831018521</v>
       </c>
@@ -3575,7 +3580,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="10" spans="1:5" ht="13" thickBot="1">
       <c r="A10" s="42">
         <v>43811.329872685186</v>
       </c>
@@ -3592,7 +3597,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="11" spans="1:5" ht="13" thickBot="1">
       <c r="A11" s="42">
         <v>43811.663518518515</v>
       </c>
@@ -3609,7 +3614,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="12" spans="1:5" ht="13" thickBot="1">
       <c r="A12" s="42">
         <v>43811.724930555552</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="13" spans="1:5" ht="13" thickBot="1">
       <c r="A13" s="42">
         <v>43811.274525462963</v>
       </c>
@@ -3660,7 +3665,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="15" spans="1:5" ht="13" thickBot="1">
       <c r="A15" s="42">
         <v>43811.589328703703</v>
       </c>
@@ -3694,154 +3699,154 @@
         <v>390</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="17" spans="1:5" ht="13" thickBot="1">
       <c r="A17" s="42">
+        <v>43815.900555555556</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>486</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="43">
+        <v>200266</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13" thickBot="1">
+      <c r="A18" s="42">
         <v>43811.364062499997</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B18" s="41" t="s">
         <v>406</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C18" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D18" s="43">
         <v>220293</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A18" s="42">
-        <v>43811.646458333336</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>414</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="D18" s="43">
-        <v>220538</v>
       </c>
       <c r="E18" s="41" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="19" spans="1:5" ht="13" thickBot="1">
       <c r="A19" s="42">
-        <v>43810.941006944442</v>
+        <v>43811.646458333336</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>428</v>
+        <v>369</v>
       </c>
       <c r="D19" s="43">
-        <v>220162</v>
+        <v>220538</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13" hidden="1" thickBot="1">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13" thickBot="1">
       <c r="A20" s="42">
-        <v>43811.529467592591</v>
+        <v>43815.276539351849</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>407</v>
+        <v>485</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D20" s="43">
-        <v>230117</v>
+        <v>230116</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>483</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13" thickBot="1">
       <c r="A21" s="42">
+        <v>43810.941006944442</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>394</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>428</v>
+      </c>
+      <c r="D21" s="43">
+        <v>220162</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="13" thickBot="1">
+      <c r="A22" s="42">
+        <v>43811.529467592591</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>407</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="D22" s="43">
+        <v>230117</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="13" thickBot="1">
+      <c r="A23" s="42">
         <v>43810.994641203702</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B23" s="41" t="s">
         <v>399</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C23" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D23" s="43">
         <v>210507</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E23" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A22" s="42">
+    <row r="24" spans="1:5" ht="13" thickBot="1">
+      <c r="A24" s="42">
         <v>43810.940752314818</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B24" s="41" t="s">
         <v>393</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C24" s="41" t="s">
         <v>427</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D24" s="43">
         <v>220180</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E24" s="41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A23" s="42">
+    <row r="25" spans="1:5" ht="13" thickBot="1">
+      <c r="A25" s="42">
         <v>43810.95484953704</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B25" s="41" t="s">
         <v>395</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C25" s="41" t="s">
         <v>373</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D25" s="43">
         <v>230201</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A24" s="42">
-        <v>43811.290995370371</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>402</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>374</v>
-      </c>
-      <c r="D24" s="43">
-        <v>230650</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A25" s="42">
-        <v>43811.644328703704</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>413</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>375</v>
-      </c>
-      <c r="D25" s="43">
-        <v>230136</v>
       </c>
       <c r="E25" s="41" t="s">
         <v>483</v>
@@ -3849,67 +3854,67 @@
     </row>
     <row r="26" spans="1:5" ht="13" thickBot="1">
       <c r="A26" s="42">
-        <v>43811.278194444443</v>
+        <v>43811.290995370371</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>169</v>
+        <v>374</v>
       </c>
       <c r="D26" s="43">
-        <v>210122</v>
+        <v>230650</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="13" hidden="1" thickBot="1">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13" thickBot="1">
       <c r="A27" s="42">
-        <v>43811.593009259261</v>
+        <v>43811.644328703704</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D27" s="43">
-        <v>220332</v>
+        <v>230136</v>
       </c>
       <c r="E27" s="41" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13" hidden="1" thickBot="1">
+    <row r="28" spans="1:5" ht="13" thickBot="1">
       <c r="A28" s="42">
-        <v>43812.001504629632</v>
+        <v>43811.278194444443</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>431</v>
+        <v>169</v>
       </c>
       <c r="D28" s="43">
-        <v>210870</v>
+        <v>210122</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="13" hidden="1" thickBot="1">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13" thickBot="1">
       <c r="A29" s="42">
-        <v>43812.993495370371</v>
+        <v>43811.593009259261</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D29" s="43">
-        <v>220200</v>
+        <v>220332</v>
       </c>
       <c r="E29" s="41" t="s">
         <v>483</v>
@@ -3917,33 +3922,33 @@
     </row>
     <row r="30" spans="1:5" ht="13" thickBot="1">
       <c r="A30" s="42">
-        <v>43810.940370370372</v>
+        <v>43812.001504629632</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>392</v>
+        <v>421</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>358</v>
+        <v>431</v>
       </c>
       <c r="D30" s="43">
-        <v>210133</v>
+        <v>210870</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="13" hidden="1" thickBot="1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="13" thickBot="1">
       <c r="A31" s="42">
-        <v>43813.803784722222</v>
+        <v>43812.993495370371</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D31" s="43">
-        <v>210864</v>
+        <v>220200</v>
       </c>
       <c r="E31" s="41" t="s">
         <v>483</v>
@@ -3951,16 +3956,16 @@
     </row>
     <row r="32" spans="1:5" ht="13" thickBot="1">
       <c r="A32" s="42">
-        <v>43811.784224537034</v>
+        <v>43810.940370370372</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>66</v>
+        <v>358</v>
       </c>
       <c r="D32" s="43">
-        <v>200183</v>
+        <v>210133</v>
       </c>
       <c r="E32" s="41" t="s">
         <v>390</v>
@@ -3968,80 +3973,109 @@
     </row>
     <row r="33" spans="1:5" ht="13" thickBot="1">
       <c r="A33" s="42">
+        <v>43813.803784722222</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33" s="43">
+        <v>210864</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="13" thickBot="1">
+      <c r="A34" s="42">
+        <v>43811.784224537034</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="43">
+        <v>200183</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13" thickBot="1">
+      <c r="A35" s="42">
         <v>43810.963425925926</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B35" s="41" t="s">
         <v>396</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C35" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D35" s="43">
         <v>210160</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E35" s="41" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A34" s="42">
-        <v>43811.701585648145</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>416</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>382</v>
-      </c>
-      <c r="D34" s="43">
-        <v>220875</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="13" hidden="1" thickBot="1">
-      <c r="A35" s="42">
-        <v>43814.732453703706</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>426</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="D35" s="43">
-        <v>220351</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13" thickBot="1">
       <c r="A36" s="42">
+        <v>43811.701585648145</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>416</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>382</v>
+      </c>
+      <c r="D36" s="43">
+        <v>220875</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="13" thickBot="1">
+      <c r="A37" s="42">
+        <v>43814.732453703706</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>426</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37" s="43">
+        <v>220351</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="13" thickBot="1">
+      <c r="A38" s="42">
         <v>43811.352013888885</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B38" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C38" s="41" t="s">
         <v>344</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D38" s="43">
         <v>200211</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E38" s="41" t="s">
         <v>390</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E36" xr:uid="{275F5ABE-440E-4960-A48D-F6ABF0A4907D}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="No"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
       <sortCondition ref="C1:C36"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
update with latest student IDs
</commit_message>
<xml_diff>
--- a/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
+++ b/rfid_reader/data/FIRST Attendance - RFID tags.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\wolfe\Documents\Misc\Personal\transfer\FIRST\Github\rfid_reader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663E5AD-C2FA-4EDE-B2BC-38C638B6CCEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F602C11-9A35-4717-A563-BB738865C44C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="810" windowWidth="28360" windowHeight="20310" tabRatio="682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3790" yWindow="3220" windowWidth="25020" windowHeight="18270" tabRatio="682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020Names" sheetId="7" r:id="rId1"/>
     <sheet name="barcodes" sheetId="8" r:id="rId2"/>
-    <sheet name="2019Names" sheetId="2" r:id="rId3"/>
-    <sheet name="Distribute these. Tags" sheetId="4" r:id="rId4"/>
+    <sheet name="Distribute these. Tags" sheetId="4" r:id="rId3"/>
+    <sheet name="2019Names" sheetId="2" r:id="rId4"/>
     <sheet name="Avail. tags" sheetId="6" r:id="rId5"/>
     <sheet name="Lost or broken tags" sheetId="3" r:id="rId6"/>
     <sheet name="Unused hello-goodbye" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2019Names'!$A$1:$D$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2019Names'!$A$1:$D$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020Names'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">barcodes!$A$1:$E$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="504">
   <si>
     <t>RFID</t>
   </si>
@@ -1415,9 +1416,6 @@
     <t>22wul@rvilleschools.org</t>
   </si>
   <si>
-    <t xml:space="preserve">Raman, Shweta </t>
-  </si>
-  <si>
     <t xml:space="preserve">Papa, Sofia </t>
   </si>
   <si>
@@ -1427,9 +1425,6 @@
     <t>D’Amico, Emmy</t>
   </si>
   <si>
-    <t>Seshadri, Madhumita</t>
-  </si>
-  <si>
     <t>Block, Nicole</t>
   </si>
   <si>
@@ -1593,6 +1588,63 @@
   </si>
   <si>
     <t>constancemehl@gmail.com</t>
+  </si>
+  <si>
+    <t>Mehl, Bill</t>
+  </si>
+  <si>
+    <t>Heulitt, Anthony</t>
+  </si>
+  <si>
+    <t>Brady, Matthew</t>
+  </si>
+  <si>
+    <t>Caputo, Michael</t>
+  </si>
+  <si>
+    <t>Banziger, Chris</t>
+  </si>
+  <si>
+    <t>Kovacs, Stephanie</t>
+  </si>
+  <si>
+    <t>Papa, Kristina</t>
+  </si>
+  <si>
+    <t>David, Stephen</t>
+  </si>
+  <si>
+    <t>Falk, Josh</t>
+  </si>
+  <si>
+    <t>Falk, Erica</t>
+  </si>
+  <si>
+    <t>iphone11 worked - semi transparent case</t>
+  </si>
+  <si>
+    <t>iPhone 10 worked - w otterbox</t>
+  </si>
+  <si>
+    <t>iPhone XR - clear case</t>
+  </si>
+  <si>
+    <t>Iphone 8 - semi-transparent</t>
+  </si>
+  <si>
+    <t>iphone 10S - carbon fiver looking case</t>
+  </si>
+  <si>
+    <t>Iphone 6S - rubbery</t>
+  </si>
+  <si>
+    <t>needs new tag</t>
+  </si>
+  <si>
+    <t>Harris, Zach+C51</t>
+  </si>
+  <si>
+    <t>999</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1725,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1692,8 +1744,26 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1716,11 +1786,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1811,10 +1901,53 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2129,19 +2262,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034DEED4-63E0-48DE-BBAF-9D5EE0076752}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" style="40" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="85.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="131.453125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="85.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="131.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -2161,7 +2294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="37.5">
+    <row r="2" spans="1:5" ht="38.25">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -2269,9 +2402,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="37.5">
+    <row r="8" spans="1:5" ht="38.25">
       <c r="A8" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B8" s="39" t="str">
         <f>IF(ISNA(VLOOKUP(C8, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C8, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2291,9 +2424,9 @@
       <c r="A9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="39" t="str">
+      <c r="B9" s="39">
         <f>IF(ISNA(VLOOKUP(C9, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C9, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>220391</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>348</v>
@@ -2306,12 +2439,12 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="47" t="s">
-        <v>439</v>
-      </c>
-      <c r="B10" s="39" t="str">
+      <c r="A10" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="B10" s="39">
         <f>IF(ISNA(VLOOKUP(C10, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C10, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>220058</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>284</v>
@@ -2323,13 +2456,13 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14">
+    <row r="11" spans="1:5" ht="14.25">
       <c r="A11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="39" t="str">
+      <c r="B11" s="39">
         <f>IF(ISNA(VLOOKUP(C11, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C11, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>200005</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>57</v>
@@ -2341,7 +2474,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25">
+    <row r="12" spans="1:5" ht="25.5">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -2359,7 +2492,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="50">
+    <row r="13" spans="1:5" ht="51">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -2377,13 +2510,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="75">
+    <row r="14" spans="1:5" ht="76.5">
       <c r="A14" t="s">
         <v>303</v>
       </c>
-      <c r="B14" s="39" t="str">
+      <c r="B14" s="39">
         <f>IF(ISNA(VLOOKUP(C14, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C14, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>210205</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>350</v>
@@ -2395,13 +2528,13 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="25">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="25.5">
       <c r="A15" t="s">
         <v>317</v>
       </c>
-      <c r="B15" s="39" t="str">
+      <c r="B15" s="39">
         <f>IF(ISNA(VLOOKUP(C15, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C15, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>200049</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>58</v>
@@ -2421,8 +2554,8 @@
         <f>IF(ISNA(VLOOKUP(C16, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C16, barcodes!$C$2:$D$71,2, FALSE))</f>
         <v/>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>175</v>
+      <c r="C16" s="36" t="s">
+        <v>502</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>191</v>
@@ -2503,7 +2636,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="62.5">
+    <row r="21" spans="1:5" ht="63.75">
       <c r="A21" t="s">
         <v>314</v>
       </c>
@@ -2523,7 +2656,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B22" s="39">
         <f>IF(ISNA(VLOOKUP(C22, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C22, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2613,7 +2746,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B27" s="39">
         <f>IF(ISNA(VLOOKUP(C27, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C27, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2633,9 +2766,9 @@
       <c r="A28" t="s">
         <v>297</v>
       </c>
-      <c r="B28" s="39" t="str">
+      <c r="B28" s="39">
         <f>IF(ISNA(VLOOKUP(C28, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C28, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>220134</v>
       </c>
       <c r="C28" s="34" t="s">
         <v>354</v>
@@ -2665,7 +2798,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="25">
+    <row r="30" spans="1:5" ht="25.5">
       <c r="A30" t="s">
         <v>306</v>
       </c>
@@ -2703,7 +2836,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B32" s="39">
         <f>IF(ISNA(VLOOKUP(C32, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C32, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2723,9 +2856,9 @@
       <c r="A33" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="39" t="str">
+      <c r="B33" s="39">
         <f>IF(ISNA(VLOOKUP(C33, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C33, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>220170</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>282</v>
@@ -2741,9 +2874,9 @@
       <c r="A34" t="s">
         <v>307</v>
       </c>
-      <c r="B34" s="39" t="str">
+      <c r="B34" s="39">
         <f>IF(ISNA(VLOOKUP(C34, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C34, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>220180</v>
       </c>
       <c r="C34" s="34" t="s">
         <v>288</v>
@@ -2793,7 +2926,7 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B37" s="39">
         <f>IF(ISNA(VLOOKUP(C37, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C37, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2809,13 +2942,13 @@
         <v>274</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25">
+    <row r="38" spans="1:5" ht="25.5">
       <c r="A38" t="s">
         <v>310</v>
       </c>
-      <c r="B38" s="39" t="str">
+      <c r="B38" s="39">
         <f>IF(ISNA(VLOOKUP(C38, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C38, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>210870</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>290</v>
@@ -2829,7 +2962,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B39" s="39">
         <f>IF(ISNA(VLOOKUP(C39, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C39, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2846,8 +2979,8 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="47" t="s">
-        <v>445</v>
+      <c r="A40" s="46" t="s">
+        <v>443</v>
       </c>
       <c r="B40" s="39">
         <f>IF(ISNA(VLOOKUP(C40, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C40, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2883,7 +3016,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B42" s="39">
         <f>IF(ISNA(VLOOKUP(C42, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C42, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -2903,8 +3036,8 @@
       <c r="A43" s="16">
         <v>49550490</v>
       </c>
-      <c r="B43" s="39">
-        <v>99</v>
+      <c r="B43" s="39" t="s">
+        <v>482</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>15</v>
@@ -2920,8 +3053,8 @@
       <c r="A44" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B44" s="39" t="s">
-        <v>484</v>
+      <c r="B44" s="68" t="s">
+        <v>503</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>
@@ -2953,7 +3086,7 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B46" s="39">
         <f>IF(ISNA(VLOOKUP(C46, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C46, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3045,9 +3178,9 @@
       <c r="A51" t="s">
         <v>324</v>
       </c>
-      <c r="B51" s="39" t="str">
+      <c r="B51" s="39">
         <f>IF(ISNA(VLOOKUP(C51, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C51, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>240554</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>362</v>
@@ -3077,13 +3210,13 @@
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="12.5" customHeight="1">
+    <row r="53" spans="1:5" ht="12.6" customHeight="1">
       <c r="A53" t="s">
         <v>326</v>
       </c>
-      <c r="B53" s="39" t="str">
+      <c r="B53" s="39">
         <f>IF(ISNA(VLOOKUP(C53, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C53, barcodes!$C$2:$D$71,2, FALSE))</f>
-        <v/>
+        <v>210247</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>363</v>
@@ -3132,7 +3265,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="44" t="s">
         <v>329</v>
       </c>
       <c r="B56" s="39">
@@ -3185,7 +3318,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25">
+    <row r="59" spans="1:5" ht="25.5">
       <c r="A59" t="s">
         <v>332</v>
       </c>
@@ -3313,7 +3446,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B66" s="39" t="str">
         <f>IF(ISNA(VLOOKUP(C66, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C66, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3331,7 +3464,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B67" s="39">
         <f>IF(ISNA(VLOOKUP(C67, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C67, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3349,7 +3482,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B68" s="39" t="str">
         <f>IF(ISNA(VLOOKUP(C68, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C68, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3365,9 +3498,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" ht="12.75" customHeight="1">
       <c r="A69" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B69" s="39">
         <f>IF(ISNA(VLOOKUP(C69, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C69, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3385,7 +3518,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B70" s="39">
         <f>IF(ISNA(VLOOKUP(C70, barcodes!$C$2:$D$71,2, FALSE)), "", VLOOKUP(C70, barcodes!$C$2:$D$71,2, FALSE))</f>
@@ -3401,7 +3534,152 @@
         <v>138</v>
       </c>
     </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>446</v>
+      </c>
+      <c r="C71" t="s">
+        <v>485</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15">
+      <c r="A72" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="C72" t="s">
+        <v>486</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>448</v>
+      </c>
+      <c r="C73" t="s">
+        <v>487</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>449</v>
+      </c>
+      <c r="C74" t="s">
+        <v>488</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>450</v>
+      </c>
+      <c r="C75" t="s">
+        <v>489</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="25.5">
+      <c r="A76" s="46" t="s">
+        <v>451</v>
+      </c>
+      <c r="C76" t="s">
+        <v>493</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="46" t="s">
+        <v>452</v>
+      </c>
+      <c r="C77" t="s">
+        <v>494</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>453</v>
+      </c>
+      <c r="C78" t="s">
+        <v>490</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" s="31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>454</v>
+      </c>
+      <c r="C79" t="s">
+        <v>491</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="63.75">
+      <c r="A80" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="C80" t="s">
+        <v>492</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="47"/>
+      <c r="C81"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{CBFD2220-F76C-490E-978A-B53D8137568B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B50:E70">
     <sortCondition ref="C50:C70"/>
   </sortState>
@@ -3412,22 +3690,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F719BBFE-2A3C-4504-AB28-C8BF6B3B6524}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.90625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.5" thickBot="1">
+    <row r="1" spans="1:5" ht="51.75" thickBot="1">
       <c r="A1" s="41" t="s">
         <v>385</v>
       </c>
@@ -3444,7 +3722,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" thickBot="1">
+    <row r="2" spans="1:5" ht="13.5" thickBot="1">
       <c r="A2" s="42">
         <v>43811.747175925928</v>
       </c>
@@ -3458,10 +3736,10 @@
         <v>230511</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13" thickBot="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" thickBot="1">
       <c r="A3" s="42">
         <v>43811.304988425924</v>
       </c>
@@ -3475,10 +3753,10 @@
         <v>230508</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13" thickBot="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" thickBot="1">
       <c r="A4" s="42">
         <v>43813.510659722226</v>
       </c>
@@ -3495,7 +3773,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13" thickBot="1">
+    <row r="5" spans="1:5" ht="13.5" thickBot="1">
       <c r="A5" s="42">
         <v>43810.982511574075</v>
       </c>
@@ -3512,7 +3790,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13" thickBot="1">
+    <row r="6" spans="1:5" ht="13.5" thickBot="1">
       <c r="A6" s="42">
         <v>43811.577881944446</v>
       </c>
@@ -3520,7 +3798,7 @@
         <v>408</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D6" s="43">
         <v>200077</v>
@@ -3529,7 +3807,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13" thickBot="1">
+    <row r="7" spans="1:5" ht="13.5" thickBot="1">
       <c r="A7" s="42">
         <v>43811.637037037035</v>
       </c>
@@ -3537,7 +3815,7 @@
         <v>412</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D7" s="43">
         <v>210150</v>
@@ -3546,536 +3824,647 @@
         <v>390</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13" thickBot="1">
-      <c r="A8" s="42">
+    <row r="8" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="43">
+        <v>200005</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="59" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="55">
+        <v>220391</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A10" s="42">
         <v>43811.633055555554</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B10" s="41" t="s">
         <v>411</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>429</v>
-      </c>
-      <c r="D8" s="43">
+      <c r="C10" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="43">
         <v>220058</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E10" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13" thickBot="1">
-      <c r="A9" s="42">
+    <row r="11" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="58" t="s">
+        <v>362</v>
+      </c>
+      <c r="D11" s="61">
+        <v>240554</v>
+      </c>
+      <c r="E11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A12" s="42">
         <v>43811.943831018521</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B12" s="41" t="s">
         <v>420</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C12" s="41" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D12" s="43">
         <v>210246</v>
       </c>
-      <c r="E9" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="13" thickBot="1">
-      <c r="A10" s="42">
+      <c r="E12" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A13" s="55"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="58" t="s">
+        <v>363</v>
+      </c>
+      <c r="D13" s="61">
+        <v>210247</v>
+      </c>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A14" s="42">
         <v>43811.329872685186</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B14" s="41" t="s">
         <v>404</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C14" s="41" t="s">
         <v>365</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D14" s="43">
         <v>230066</v>
       </c>
-      <c r="E10" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="13" thickBot="1">
-      <c r="A11" s="42">
-        <v>43811.663518518515</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>415</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>367</v>
-      </c>
-      <c r="D11" s="43">
-        <v>230076</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="13" thickBot="1">
-      <c r="A12" s="42">
-        <v>43811.724930555552</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>417</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="43">
-        <v>200806</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="13" thickBot="1">
-      <c r="A13" s="42">
-        <v>43811.274525462963</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>400</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="D13" s="43">
-        <v>220108</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="13" thickBot="1">
-      <c r="A14" s="42">
-        <v>43812.754351851851</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>422</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="43">
-        <v>210081</v>
-      </c>
       <c r="E14" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="41" t="s">
+        <v>350</v>
+      </c>
+      <c r="D15" s="43">
+        <v>210205</v>
+      </c>
+      <c r="E15" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13" thickBot="1">
-      <c r="A15" s="42">
-        <v>43811.589328703703</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>353</v>
-      </c>
-      <c r="D15" s="43">
-        <v>220127</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="13" thickBot="1">
-      <c r="A16" s="42">
-        <v>43810.988634259258</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>398</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="43">
-        <v>200201</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="13" thickBot="1">
-      <c r="A17" s="42">
-        <v>43815.900555555556</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>486</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>62</v>
+    <row r="16" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A16" s="55"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="61">
+        <v>200049</v>
+      </c>
+      <c r="E16" s="55"/>
+    </row>
+    <row r="17" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="D17" s="43">
-        <v>200266</v>
+        <v>200082</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13" thickBot="1">
+    <row r="18" spans="1:5" ht="13.5" thickBot="1">
       <c r="A18" s="42">
-        <v>43811.364062499997</v>
+        <v>43811.663518518515</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D18" s="43">
-        <v>220293</v>
+        <v>230076</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="13" thickBot="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.5" thickBot="1">
       <c r="A19" s="42">
-        <v>43811.646458333336</v>
+        <v>43811.724930555552</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>369</v>
+        <v>176</v>
       </c>
       <c r="D19" s="43">
-        <v>220538</v>
+        <v>200806</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13" thickBot="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.5" thickBot="1">
       <c r="A20" s="42">
-        <v>43815.276539351849</v>
+        <v>43811.274525462963</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>485</v>
+        <v>400</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>371</v>
+        <v>283</v>
       </c>
       <c r="D20" s="43">
-        <v>230116</v>
+        <v>220108</v>
       </c>
       <c r="E20" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A21" s="42">
+        <v>43812.754351851851</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>422</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="43">
+        <v>210081</v>
+      </c>
+      <c r="E21" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13" thickBot="1">
-      <c r="A21" s="42">
-        <v>43810.941006944442</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>394</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>428</v>
-      </c>
-      <c r="D21" s="43">
-        <v>220162</v>
-      </c>
-      <c r="E21" s="41" t="s">
+    <row r="22" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A22" s="42">
+        <v>43811.589328703703</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>353</v>
+      </c>
+      <c r="D22" s="43">
+        <v>220127</v>
+      </c>
+      <c r="E22" s="41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13" thickBot="1">
-      <c r="A22" s="42">
-        <v>43811.529467592591</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>407</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>372</v>
-      </c>
-      <c r="D22" s="43">
-        <v>230117</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="13" thickBot="1">
+    <row r="23" spans="1:5" ht="13.5" thickBot="1">
       <c r="A23" s="42">
-        <v>43810.994641203702</v>
+        <v>43810.988634259258</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="D23" s="43">
-        <v>210507</v>
+        <v>200201</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13" thickBot="1">
+    <row r="24" spans="1:5" ht="13.5" thickBot="1">
       <c r="A24" s="42">
-        <v>43810.940752314818</v>
+        <v>43815.900555555556</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>393</v>
+        <v>484</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>427</v>
+        <v>62</v>
       </c>
       <c r="D24" s="43">
-        <v>220180</v>
+        <v>200266</v>
       </c>
       <c r="E24" s="41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="13" thickBot="1">
+    <row r="25" spans="1:5" ht="13.5" thickBot="1">
       <c r="A25" s="42">
+        <v>43811.364062499997</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>406</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>368</v>
+      </c>
+      <c r="D25" s="43">
+        <v>220293</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A26" s="42">
+        <v>43811.646458333336</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>414</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>369</v>
+      </c>
+      <c r="D26" s="43">
+        <v>220538</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A27" s="42">
+        <v>43815.276539351849</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>371</v>
+      </c>
+      <c r="D27" s="43">
+        <v>230116</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A28" s="42">
+        <v>43810.941006944442</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>427</v>
+      </c>
+      <c r="D28" s="43">
+        <v>220162</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A29" s="42">
+        <v>43811.529467592591</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>407</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="D29" s="43">
+        <v>230117</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A30" s="42">
+        <v>43810.994641203702</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>399</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="43">
+        <v>210507</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A31" s="55"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="59" t="s">
+        <v>282</v>
+      </c>
+      <c r="D31" s="61">
+        <v>220170</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A32" s="42">
+        <v>43810.940752314818</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>393</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="D32" s="43">
+        <v>220180</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A33" s="42">
         <v>43810.95484953704</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B33" s="41" t="s">
         <v>395</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C33" s="41" t="s">
         <v>373</v>
       </c>
-      <c r="D25" s="43">
+      <c r="D33" s="43">
         <v>230201</v>
       </c>
-      <c r="E25" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="13" thickBot="1">
-      <c r="A26" s="42">
+      <c r="E33" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A34" s="42">
         <v>43811.290995370371</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B34" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C34" s="41" t="s">
         <v>374</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D34" s="43">
         <v>230650</v>
       </c>
-      <c r="E26" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="13" thickBot="1">
-      <c r="A27" s="42">
-        <v>43811.644328703704</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>413</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>375</v>
-      </c>
-      <c r="D27" s="43">
-        <v>230136</v>
-      </c>
-      <c r="E27" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="13" thickBot="1">
-      <c r="A28" s="42">
-        <v>43811.278194444443</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>401</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>169</v>
-      </c>
-      <c r="D28" s="43">
-        <v>210122</v>
-      </c>
-      <c r="E28" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="13" thickBot="1">
-      <c r="A29" s="42">
-        <v>43811.593009259261</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>410</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>376</v>
-      </c>
-      <c r="D29" s="43">
-        <v>220332</v>
-      </c>
-      <c r="E29" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="13" thickBot="1">
-      <c r="A30" s="42">
-        <v>43812.001504629632</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>421</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>431</v>
-      </c>
-      <c r="D30" s="43">
-        <v>210870</v>
-      </c>
-      <c r="E30" s="41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="13" thickBot="1">
-      <c r="A31" s="42">
-        <v>43812.993495370371</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>423</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>378</v>
-      </c>
-      <c r="D31" s="43">
-        <v>220200</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="13" thickBot="1">
-      <c r="A32" s="42">
-        <v>43810.940370370372</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>392</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>358</v>
-      </c>
-      <c r="D32" s="43">
-        <v>210133</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="13" thickBot="1">
-      <c r="A33" s="42">
-        <v>43813.803784722222</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>425</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>380</v>
-      </c>
-      <c r="D33" s="43">
-        <v>210864</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="13" thickBot="1">
-      <c r="A34" s="42">
-        <v>43811.784224537034</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="43">
-        <v>200183</v>
-      </c>
       <c r="E34" s="41" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="13" thickBot="1">
-      <c r="A35" s="42">
-        <v>43810.963425925926</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>396</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>173</v>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="34" t="s">
+        <v>354</v>
       </c>
       <c r="D35" s="43">
-        <v>210160</v>
+        <v>220134</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13" thickBot="1">
+    <row r="36" spans="1:5" ht="13.5" thickBot="1">
       <c r="A36" s="42">
+        <v>43811.644328703704</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D36" s="43">
+        <v>230136</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A37" s="42">
+        <v>43811.278194444443</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>401</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="43">
+        <v>210122</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A38" s="42">
+        <v>43811.593009259261</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>376</v>
+      </c>
+      <c r="D38" s="43">
+        <v>220332</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="56">
+        <v>43812.001504629632</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="C39" s="60" t="s">
+        <v>290</v>
+      </c>
+      <c r="D39" s="63">
+        <v>210870</v>
+      </c>
+      <c r="E39" s="60" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="56">
+        <v>43812.993495370371</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>423</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="D40" s="62">
+        <v>220200</v>
+      </c>
+      <c r="E40" s="60" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="56">
+        <v>43810.940370370372</v>
+      </c>
+      <c r="B41" s="57" t="s">
+        <v>392</v>
+      </c>
+      <c r="C41" s="60" t="s">
+        <v>358</v>
+      </c>
+      <c r="D41" s="62">
+        <v>210133</v>
+      </c>
+      <c r="E41" s="57" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="64">
+        <v>43813.803784722222</v>
+      </c>
+      <c r="B42" s="65" t="s">
+        <v>425</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="D42" s="66">
+        <v>210864</v>
+      </c>
+      <c r="E42" s="65" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A43" s="56">
+        <v>43811.784224537034</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>419</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="62">
+        <v>200183</v>
+      </c>
+      <c r="E43" s="57" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A44" s="56">
+        <v>43810.963425925926</v>
+      </c>
+      <c r="B44" s="57" t="s">
+        <v>396</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="43">
+        <v>210160</v>
+      </c>
+      <c r="E44" s="57" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A45" s="56">
         <v>43811.701585648145</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B45" s="57" t="s">
         <v>416</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C45" s="41" t="s">
         <v>382</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D45" s="43">
         <v>220875</v>
       </c>
-      <c r="E36" s="41" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="13" thickBot="1">
-      <c r="A37" s="42">
+      <c r="E45" s="41" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A46" s="56">
         <v>43814.732453703706</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B46" s="57" t="s">
         <v>426</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C46" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D46" s="43">
         <v>220351</v>
       </c>
-      <c r="E37" s="41" t="s">
+      <c r="E46" s="41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13" thickBot="1">
-      <c r="A38" s="42">
+    <row r="47" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A47" s="56">
         <v>43811.352013888885</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B47" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C47" s="67" t="s">
         <v>344</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D47" s="43">
         <v>200211</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E47" s="41" t="s">
         <v>390</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E36" xr:uid="{275F5ABE-440E-4960-A48D-F6ABF0A4907D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">
       <sortCondition ref="C1:C36"/>
     </sortState>
   </autoFilter>
@@ -4085,6 +4474,556 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229FC06A-43DC-4B28-BD17-66C7FA82B8B7}">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="48" customFormat="1">
+      <c r="A2" s="48">
+        <v>232</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="48" customFormat="1">
+      <c r="A3" s="48">
+        <v>234</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="48" customFormat="1">
+      <c r="A4" s="48">
+        <v>235</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="48" customFormat="1">
+      <c r="A5" s="48">
+        <v>236</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="48" customFormat="1">
+      <c r="A6" s="48">
+        <v>237</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="48" customFormat="1">
+      <c r="A7" s="48">
+        <v>238</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>365</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="48" customFormat="1">
+      <c r="A8" s="48">
+        <v>239</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="48" customFormat="1">
+      <c r="A9" s="48">
+        <v>240</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="48" customFormat="1">
+      <c r="A10" s="48">
+        <v>241</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>242</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="48" customFormat="1">
+      <c r="A12" s="48">
+        <v>243</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="48" customFormat="1">
+      <c r="A13" s="48">
+        <v>244</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="48" customFormat="1">
+      <c r="A14" s="48">
+        <v>245</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="48" customFormat="1">
+      <c r="A15" s="48">
+        <v>246</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>373</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="48" customFormat="1">
+      <c r="A16" s="48">
+        <v>247</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="48" customFormat="1">
+      <c r="A17" s="48">
+        <v>248</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>337</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="48" customFormat="1">
+      <c r="A18" s="48">
+        <v>249</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>338</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>300</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="48" customFormat="1">
+      <c r="A20" s="48">
+        <v>301</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>432</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>378</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>302</v>
+      </c>
+      <c r="B21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="48" customFormat="1">
+      <c r="A22" s="48">
+        <v>303</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="48" customFormat="1">
+      <c r="A23" s="48">
+        <v>304</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="13.5" thickBot="1">
+      <c r="B24"/>
+      <c r="C24" s="33"/>
+    </row>
+    <row r="25" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A25">
+        <v>305</v>
+      </c>
+      <c r="B25" t="s">
+        <v>436</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A26">
+        <v>306</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A27">
+        <v>307</v>
+      </c>
+      <c r="B27" t="s">
+        <v>438</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A28">
+        <v>308</v>
+      </c>
+      <c r="B28" t="s">
+        <v>439</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A29">
+        <v>309</v>
+      </c>
+      <c r="B29" t="s">
+        <v>440</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A30">
+        <v>310</v>
+      </c>
+      <c r="B30" t="s">
+        <v>441</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A31">
+        <v>311</v>
+      </c>
+      <c r="B31" t="s">
+        <v>442</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A32">
+        <v>312</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A33">
+        <v>313</v>
+      </c>
+      <c r="B33" t="s">
+        <v>444</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A34">
+        <v>314</v>
+      </c>
+      <c r="B34" t="s">
+        <v>445</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>315</v>
+      </c>
+      <c r="B36" t="s">
+        <v>446</v>
+      </c>
+      <c r="C36" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="48" customFormat="1">
+      <c r="A37" s="48">
+        <v>316</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>447</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>317</v>
+      </c>
+      <c r="B38" t="s">
+        <v>448</v>
+      </c>
+      <c r="C38" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>318</v>
+      </c>
+      <c r="B39" t="s">
+        <v>449</v>
+      </c>
+      <c r="C39" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>319</v>
+      </c>
+      <c r="B40" t="s">
+        <v>450</v>
+      </c>
+      <c r="C40" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="52" customFormat="1">
+      <c r="A41" s="52">
+        <v>320</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="48" customFormat="1">
+      <c r="A42" s="48">
+        <v>321</v>
+      </c>
+      <c r="B42" s="50" t="s">
+        <v>452</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>322</v>
+      </c>
+      <c r="B43" t="s">
+        <v>453</v>
+      </c>
+      <c r="C43" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>323</v>
+      </c>
+      <c r="B44" t="s">
+        <v>454</v>
+      </c>
+      <c r="C44" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="48" customFormat="1">
+      <c r="A45" s="48">
+        <v>324</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>455</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>492</v>
+      </c>
+      <c r="E45" s="48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>325</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="C46" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="48" customFormat="1">
+      <c r="A47" s="48">
+        <v>326</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="E47" s="48" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="54" customFormat="1">
+      <c r="A48" s="54">
+        <v>327</v>
+      </c>
+      <c r="B48" s="54" t="s">
+        <v>458</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C23">
+    <sortCondition ref="C2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
@@ -4093,12 +5032,12 @@
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="85.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="131.453125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="131.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
@@ -4115,7 +5054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.5">
+    <row r="2" spans="1:4" ht="12.75">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
@@ -4129,7 +5068,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5">
+    <row r="3" spans="1:4" ht="38.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -4143,7 +5082,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.5">
+    <row r="4" spans="1:4" ht="12.75">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -4157,7 +5096,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.5">
+    <row r="5" spans="1:4" ht="12.75">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -4171,7 +5110,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.5">
+    <row r="6" spans="1:4" ht="12.75">
       <c r="A6" t="s">
         <v>295</v>
       </c>
@@ -4199,7 +5138,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.5">
+    <row r="8" spans="1:4" ht="12.75">
       <c r="A8" s="18" t="s">
         <v>312</v>
       </c>
@@ -4213,7 +5152,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="12" t="s">
         <v>341</v>
       </c>
@@ -4227,7 +5166,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.5">
+    <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -4241,7 +5180,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.5">
+    <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="18" t="s">
         <v>54</v>
       </c>
@@ -4255,7 +5194,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="37.5">
+    <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="13" t="s">
         <v>50</v>
       </c>
@@ -4269,7 +5208,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.5">
+    <row r="13" spans="1:4" ht="12.75">
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
@@ -4283,7 +5222,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.5">
+    <row r="14" spans="1:4" ht="12.75">
       <c r="A14" s="26" t="s">
         <v>293</v>
       </c>
@@ -4297,7 +5236,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14">
+    <row r="15" spans="1:4" ht="14.25">
       <c r="A15" s="11" t="s">
         <v>30</v>
       </c>
@@ -4311,7 +5250,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="25">
+    <row r="16" spans="1:4" ht="25.5">
       <c r="A16" t="s">
         <v>320</v>
       </c>
@@ -4325,7 +5264,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="50">
+    <row r="17" spans="1:4" ht="51">
       <c r="A17" t="s">
         <v>301</v>
       </c>
@@ -4339,7 +5278,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.5">
+    <row r="18" spans="1:4" ht="12.75">
       <c r="A18" s="1" t="s">
         <v>340</v>
       </c>
@@ -4353,7 +5292,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="75">
+    <row r="19" spans="1:4" ht="76.5">
       <c r="A19" t="s">
         <v>303</v>
       </c>
@@ -4367,7 +5306,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="25">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="25.5">
       <c r="A20" t="s">
         <v>317</v>
       </c>
@@ -4381,7 +5320,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.5">
+    <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="13" t="s">
         <v>51</v>
       </c>
@@ -4395,7 +5334,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.5">
+    <row r="22" spans="1:4" ht="12.75">
       <c r="A22" t="s">
         <v>318</v>
       </c>
@@ -4409,7 +5348,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.5">
+    <row r="23" spans="1:4" ht="12.75">
       <c r="A23" t="s">
         <v>319</v>
       </c>
@@ -4423,7 +5362,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="50">
+    <row r="24" spans="1:4" ht="51">
       <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
@@ -4437,7 +5376,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.5">
+    <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="26" t="s">
         <v>35</v>
       </c>
@@ -4451,7 +5390,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.5">
+    <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -4465,7 +5404,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.5">
+    <row r="27" spans="1:4" ht="12.75">
       <c r="A27" s="18" t="s">
         <v>313</v>
       </c>
@@ -4479,7 +5418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="62.5">
+    <row r="28" spans="1:4" ht="63.75">
       <c r="A28" t="s">
         <v>314</v>
       </c>
@@ -4493,7 +5432,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="12.5">
+    <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="13" t="s">
         <v>52</v>
       </c>
@@ -4507,7 +5446,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.5">
+    <row r="30" spans="1:4" ht="12.75">
       <c r="A30" t="s">
         <v>323</v>
       </c>
@@ -4521,7 +5460,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.5">
+    <row r="31" spans="1:4" ht="12.75">
       <c r="A31" s="13" t="s">
         <v>53</v>
       </c>
@@ -4535,7 +5474,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.5">
+    <row r="32" spans="1:4" ht="12.75">
       <c r="A32" t="s">
         <v>299</v>
       </c>
@@ -4549,7 +5488,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="12.5">
+    <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="11" t="s">
         <v>33</v>
       </c>
@@ -4563,7 +5502,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.5">
+    <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="12" t="s">
         <v>26</v>
       </c>
@@ -4577,7 +5516,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.5">
+    <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="14" t="s">
         <v>34</v>
       </c>
@@ -4591,7 +5530,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.5">
+    <row r="36" spans="1:4" ht="12.75">
       <c r="A36" t="s">
         <v>297</v>
       </c>
@@ -4605,7 +5544,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="12.5">
+    <row r="37" spans="1:4" ht="12.75">
       <c r="A37" t="s">
         <v>316</v>
       </c>
@@ -4619,7 +5558,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="12.5">
+    <row r="38" spans="1:4" ht="12.75">
       <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
@@ -4633,7 +5572,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="12.5">
+    <row r="39" spans="1:4" ht="12.75">
       <c r="A39" s="11" t="s">
         <v>37</v>
       </c>
@@ -4647,7 +5586,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="12.5">
+    <row r="40" spans="1:4" ht="12.75">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -4661,7 +5600,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="25">
+    <row r="41" spans="1:4" ht="25.5">
       <c r="A41" t="s">
         <v>306</v>
       </c>
@@ -4675,7 +5614,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.5">
+    <row r="42" spans="1:4" ht="12.75">
       <c r="A42" t="s">
         <v>298</v>
       </c>
@@ -4689,7 +5628,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="12.5">
+    <row r="43" spans="1:4" ht="12.75">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -4843,7 +5782,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="12.5">
+    <row r="54" spans="1:4" ht="12.75">
       <c r="A54" t="s">
         <v>322</v>
       </c>
@@ -4857,7 +5796,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="12.5">
+    <row r="55" spans="1:4" ht="12.75">
       <c r="A55" t="s">
         <v>315</v>
       </c>
@@ -4871,7 +5810,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="12.5">
+    <row r="56" spans="1:4" ht="12.75">
       <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
@@ -4885,7 +5824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="25">
+    <row r="57" spans="1:4" ht="25.5">
       <c r="A57" t="s">
         <v>310</v>
       </c>
@@ -4899,7 +5838,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="12.5">
+    <row r="58" spans="1:4" ht="12.75">
       <c r="A58" t="s">
         <v>309</v>
       </c>
@@ -4913,7 +5852,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="12.5">
+    <row r="59" spans="1:4" ht="12.75">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
@@ -4927,7 +5866,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="12.5">
+    <row r="60" spans="1:4" ht="12.75">
       <c r="A60" s="1" t="s">
         <v>45</v>
       </c>
@@ -4941,7 +5880,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="25">
+    <row r="61" spans="1:4" ht="25.5">
       <c r="A61" t="s">
         <v>296</v>
       </c>
@@ -4955,7 +5894,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="12.5">
+    <row r="62" spans="1:4" ht="12.75">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
@@ -4969,7 +5908,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="12.5">
+    <row r="63" spans="1:4" ht="12.75">
       <c r="A63" s="1" t="s">
         <v>24</v>
       </c>
@@ -4983,7 +5922,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12.5">
+    <row r="64" spans="1:4" ht="12.75">
       <c r="A64" s="14" t="s">
         <v>343</v>
       </c>
@@ -5053,7 +5992,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="12.5">
+    <row r="69" spans="1:4" ht="12.75">
       <c r="A69" s="12" t="s">
         <v>47</v>
       </c>
@@ -5067,7 +6006,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="12.5">
+    <row r="70" spans="1:4" ht="12.75">
       <c r="A70" s="11" t="s">
         <v>22</v>
       </c>
@@ -5099,16 +6038,16 @@
       <c r="A73" s="11"/>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:4" ht="12.5">
+    <row r="74" spans="1:4" ht="12.75">
       <c r="A74" s="11"/>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:4" ht="12.5"/>
-    <row r="76" spans="1:4" ht="12.5"/>
-    <row r="77" spans="1:4" ht="12.5"/>
-    <row r="78" spans="1:4" ht="12.5"/>
-    <row r="79" spans="1:4" ht="12.5"/>
-    <row r="80" spans="1:4" ht="12.5"/>
+    <row r="75" spans="1:4" ht="12.75"/>
+    <row r="76" spans="1:4" ht="12.75"/>
+    <row r="77" spans="1:4" ht="12.75"/>
+    <row r="78" spans="1:4" ht="12.75"/>
+    <row r="79" spans="1:4" ht="12.75"/>
+    <row r="80" spans="1:4" ht="12.75"/>
   </sheetData>
   <autoFilter ref="A1:D71" xr:uid="{08B00641-7E2D-4DEA-AC7A-FFE6E7706878}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
@@ -5121,401 +6060,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229FC06A-43DC-4B28-BD17-66C7FA82B8B7}">
-  <dimension ref="A1:C34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
-  <cols>
-    <col min="2" max="2" width="10.26953125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>232</v>
-      </c>
-      <c r="B2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>235</v>
-      </c>
-      <c r="B4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>236</v>
-      </c>
-      <c r="B5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>237</v>
-      </c>
-      <c r="B6" t="s">
-        <v>326</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>238</v>
-      </c>
-      <c r="B7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>239</v>
-      </c>
-      <c r="B8" t="s">
-        <v>328</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>240</v>
-      </c>
-      <c r="B9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>241</v>
-      </c>
-      <c r="B10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>242</v>
-      </c>
-      <c r="B11" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>243</v>
-      </c>
-      <c r="B12" t="s">
-        <v>332</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>244</v>
-      </c>
-      <c r="B13" t="s">
-        <v>333</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>245</v>
-      </c>
-      <c r="B14" t="s">
-        <v>334</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>246</v>
-      </c>
-      <c r="B15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>247</v>
-      </c>
-      <c r="B16" t="s">
-        <v>336</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>248</v>
-      </c>
-      <c r="B17" t="s">
-        <v>337</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>249</v>
-      </c>
-      <c r="B18" t="s">
-        <v>338</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>300</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>433</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>301</v>
-      </c>
-      <c r="B20" t="s">
-        <v>434</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>302</v>
-      </c>
-      <c r="B21" t="s">
-        <v>435</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>303</v>
-      </c>
-      <c r="B22" t="s">
-        <v>436</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>304</v>
-      </c>
-      <c r="B23" t="s">
-        <v>437</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="13" thickBot="1">
-      <c r="B24"/>
-      <c r="C24" s="33"/>
-    </row>
-    <row r="25" spans="1:3" ht="13" thickBot="1">
-      <c r="A25">
-        <v>305</v>
-      </c>
-      <c r="B25" t="s">
-        <v>438</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="13" thickBot="1">
-      <c r="A26">
-        <v>306</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>439</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="13" thickBot="1">
-      <c r="A27">
-        <v>307</v>
-      </c>
-      <c r="B27" t="s">
-        <v>440</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="13" thickBot="1">
-      <c r="A28">
-        <v>308</v>
-      </c>
-      <c r="B28" t="s">
-        <v>441</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="13" thickBot="1">
-      <c r="A29">
-        <v>309</v>
-      </c>
-      <c r="B29" t="s">
-        <v>442</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="13" thickBot="1">
-      <c r="A30">
-        <v>310</v>
-      </c>
-      <c r="B30" t="s">
-        <v>443</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="13" thickBot="1">
-      <c r="A31">
-        <v>311</v>
-      </c>
-      <c r="B31" t="s">
-        <v>444</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="13" thickBot="1">
-      <c r="A32">
-        <v>312</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>445</v>
-      </c>
-      <c r="C32" s="46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="13" thickBot="1">
-      <c r="A33">
-        <v>313</v>
-      </c>
-      <c r="B33" t="s">
-        <v>446</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="13" thickBot="1">
-      <c r="A34">
-        <v>314</v>
-      </c>
-      <c r="B34" t="s">
-        <v>447</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>344</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C23">
-    <sortCondition ref="C2"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90371E08-1F3F-42FF-B479-1FD1C921154F}">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -5556,116 +6109,12 @@
     <row r="4" spans="1:3">
       <c r="B4" s="18"/>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>315</v>
-      </c>
-      <c r="B6" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>316</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>317</v>
-      </c>
-      <c r="B8" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>318</v>
-      </c>
-      <c r="B9" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>319</v>
-      </c>
-      <c r="B10" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>320</v>
-      </c>
-      <c r="B11" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>321</v>
-      </c>
-      <c r="B12" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>322</v>
-      </c>
-      <c r="B13" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>323</v>
-      </c>
-      <c r="B14" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>324</v>
-      </c>
-      <c r="B15" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>325</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>326</v>
-      </c>
-      <c r="B17" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>327</v>
-      </c>
-      <c r="B18" t="s">
-        <v>460</v>
-      </c>
-    </row>
     <row r="19" spans="1:2">
       <c r="A19">
         <v>328</v>
       </c>
       <c r="B19" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5673,7 +6122,7 @@
         <v>329</v>
       </c>
       <c r="B20" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5681,7 +6130,7 @@
         <v>330</v>
       </c>
       <c r="B21" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5689,7 +6138,7 @@
         <v>331</v>
       </c>
       <c r="B22" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5697,7 +6146,7 @@
         <v>332</v>
       </c>
       <c r="B23" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5705,7 +6154,7 @@
         <v>333</v>
       </c>
       <c r="B24" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -5713,7 +6162,7 @@
         <v>334</v>
       </c>
       <c r="B25" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5721,7 +6170,7 @@
         <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5729,7 +6178,7 @@
         <v>336</v>
       </c>
       <c r="B27" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5737,7 +6186,7 @@
         <v>337</v>
       </c>
       <c r="B28" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5745,7 +6194,7 @@
         <v>338</v>
       </c>
       <c r="B29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5753,7 +6202,7 @@
         <v>339</v>
       </c>
       <c r="B30" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5761,7 +6210,7 @@
         <v>340</v>
       </c>
       <c r="B31" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5769,7 +6218,7 @@
         <v>341</v>
       </c>
       <c r="B32" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5777,7 +6226,7 @@
         <v>342</v>
       </c>
       <c r="B33" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5785,7 +6234,7 @@
         <v>343</v>
       </c>
       <c r="B34" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -5793,7 +6242,7 @@
         <v>344</v>
       </c>
       <c r="B35" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5801,7 +6250,7 @@
         <v>345</v>
       </c>
       <c r="B36" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5809,7 +6258,7 @@
         <v>346</v>
       </c>
       <c r="B37" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5817,7 +6266,7 @@
         <v>347</v>
       </c>
       <c r="B38" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5825,7 +6274,7 @@
         <v>348</v>
       </c>
       <c r="B39" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -5833,7 +6282,7 @@
         <v>349</v>
       </c>
       <c r="B40" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -5849,9 +6298,9 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5875,16 +6324,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B571F4-9364-46F7-82CE-0B9371F3638F}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B42"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="57.81640625" customWidth="1"/>
-    <col min="2" max="2" width="82.81640625" customWidth="1"/>
+    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="82.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5903,7 +6352,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="25">
+    <row r="29" spans="1:2" ht="25.5">
       <c r="A29" s="3" t="s">
         <v>206</v>
       </c>
@@ -5933,7 +6382,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="50">
+    <row r="38" spans="1:2" ht="51">
       <c r="A38" s="17" t="s">
         <v>98</v>
       </c>
@@ -5957,176 +6406,100 @@
       <c r="A57" s="1"/>
       <c r="B57" s="27"/>
     </row>
-    <row r="58" spans="1:2" ht="13">
+    <row r="58" spans="1:2">
       <c r="A58" s="32" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.5">
-      <c r="A60" s="24" t="s">
-        <v>115</v>
+      <c r="A59" s="21"/>
+      <c r="B59" s="23"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="15" t="s">
-        <v>116</v>
+        <v>280</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="62.5">
-      <c r="A64" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="25">
-      <c r="A65" s="1" t="s">
-        <v>113</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="25.5">
+      <c r="A65" s="30" t="s">
+        <v>96</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="37.5">
-      <c r="A67" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="25">
-      <c r="A69" s="30" t="s">
-        <v>96</v>
+      <c r="A66" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="25.5">
+      <c r="A68" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="B70" s="29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="63.75">
+      <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="38.25">
       <c r="A71" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="31" t="s">
-        <v>135</v>
+        <v>162</v>
+      </c>
+      <c r="B71" s="23" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B72" s="31" t="s">
-        <v>273</v>
+        <v>90</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B73" s="31" t="s">
-        <v>129</v>
+      <c r="A73" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
-        <v>161</v>
+      <c r="A74" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="62.5">
-      <c r="A75" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="37.5">
-      <c r="A76" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B79" s="23" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>